<commit_message>
[10-issue0005_ucv03] Update README.md and modify resource.
</commit_message>
<xml_diff>
--- a/Resources/README/README_Resources.xlsx
+++ b/Resources/README/README_Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\CSC_MS\Resources\README\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C389D20C-7ED3-4EFD-AD74-B6F38F04DC6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F1E24D-332A-4F07-97D0-DAE6884A97D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13545" xr2:uid="{5FC90DE4-2FBD-4B96-ADE9-01AE3F36C35E}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="66">
   <si>
     <t>SyRS</t>
     <phoneticPr fontId="2"/>
@@ -202,76 +202,53 @@
     <t>NUCLEO-G0B1RE</t>
   </si>
   <si>
-    <t>Link</t>
-  </si>
-  <si>
-    <t>Flash</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>Stock</t>
   </si>
   <si>
-    <t>Delivery(day)</t>
-  </si>
-  <si>
     <t>NUCLEO-C031C6</t>
   </si>
   <si>
-    <t>https://www.marutsu.co.jp/pc/i/43347410/</t>
-  </si>
-  <si>
-    <t>https://www.marutsu.co.jp/pc/i/40719714/</t>
-  </si>
-  <si>
     <t>NUCLEO-C071RB</t>
   </si>
   <si>
-    <t>https://www.marutsu.co.jp/GoodsDetail.jsp?q=NUCLEO-C071RB&amp;salesGoodsCode=48382034&amp;shopNo=3</t>
-  </si>
-  <si>
-    <t>https://www.marutsu.co.jp/pc/i/13537476/</t>
-  </si>
-  <si>
     <t>NUCLEO-F030R8</t>
   </si>
   <si>
     <t>NUCLEO-F070RB</t>
   </si>
   <si>
-    <t>https://www.marutsu.co.jp/pc/i/13537479/</t>
-  </si>
-  <si>
-    <t>https://www.marutsu.co.jp/pc/i/13537480/</t>
-  </si>
-  <si>
     <t>NUCLEO-F072RB</t>
   </si>
   <si>
     <t>NUCLEO-F091RC</t>
   </si>
   <si>
-    <t>https://www.marutsu.co.jp/pc/i/13537481/</t>
-  </si>
-  <si>
     <t>NUCLEO-G070RB</t>
   </si>
   <si>
-    <t>https://www.marutsu.co.jp/pc/i/32060905/</t>
-  </si>
-  <si>
     <t>NUCLEO-G071RB</t>
   </si>
   <si>
-    <t>https://www.marutsu.co.jp/pc/i/31819503/</t>
-  </si>
-  <si>
     <t>EVB</t>
+  </si>
+  <si>
+    <t>https://www.marutsu.co.jp</t>
+  </si>
+  <si>
+    <t>Delivery
+(day)</t>
+  </si>
+  <si>
+    <t>Flash
+(KB)</t>
+  </si>
+  <si>
+    <t>Ram
+(KB)</t>
+  </si>
+  <si>
+    <t>Price
+(Yen)</t>
   </si>
 </sst>
 </file>
@@ -281,7 +258,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,8 +339,16 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,6 +373,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="55">
     <border>
@@ -1012,7 +1003,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1322,7 +1313,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1331,47 +1361,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1479,7 +1479,8 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Flash</c:v>
+                  <c:v>Flash
+(KB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1596,7 +1597,8 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ram</c:v>
+                  <c:v>Ram
+(KB)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1865,6 +1867,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1931230720"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2077,22 +2080,22 @@
             <c:numRef>
               <c:f>Marketshare!$C$6:$G$6</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18.8</c:v>
+                  <c:v>0.188</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.8</c:v>
+                  <c:v>0.17800000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.7</c:v>
+                  <c:v>0.16699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.8</c:v>
+                  <c:v>0.11800000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2339,7 +2342,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3682,50 +3685,6 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>24914</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>46021</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="図 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD79F4D8-89CB-42A9-ADEF-3AA2EFDADE9C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4876800" y="4953000"/>
-          <a:ext cx="6120914" cy="3475021"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4028,10 +3987,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80D6046F-E043-414C-A439-6B06F250CAC0}">
-  <dimension ref="B2:H12"/>
+  <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4045,258 +4004,235 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
-      <c r="B3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H3" t="s">
+    <row r="3" spans="2:8" ht="30">
+      <c r="B3" s="123" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="124" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="124" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="124" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="124" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" s="123" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="122" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="122">
         <v>32</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="122">
         <v>12</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="122">
         <v>2197</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="122">
         <v>5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="122">
         <v>584</v>
       </c>
-      <c r="H4" s="121" t="s">
-        <v>58</v>
-      </c>
+      <c r="H4" s="105"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C5">
+      <c r="B5" s="122" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="122">
         <v>128</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="122">
         <v>24</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="122">
         <v>2242</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="122">
         <v>5</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="122">
         <v>136</v>
       </c>
-      <c r="H5" s="121" t="s">
-        <v>61</v>
-      </c>
+      <c r="H5" s="105"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6">
+      <c r="B6" s="122" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="122">
         <v>64</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="122">
         <v>8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="122">
         <v>2201</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="122">
         <v>5</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="122">
         <v>663</v>
       </c>
-      <c r="H6" s="121" t="s">
-        <v>62</v>
-      </c>
+      <c r="H6" s="105"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7">
+      <c r="B7" s="122" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="122">
         <v>128</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="122">
         <v>16</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="122">
         <v>2201</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="122">
         <v>5</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="122">
         <v>71</v>
       </c>
-      <c r="H7" s="121" t="s">
-        <v>65</v>
-      </c>
+      <c r="H7" s="105"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="122" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="122">
         <v>128</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="122">
         <v>16</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="122">
         <v>2201</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="122">
         <v>5</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="122">
         <v>304</v>
       </c>
-      <c r="H8" s="121" t="s">
-        <v>66</v>
-      </c>
+      <c r="H8" s="105"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="122" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="122">
         <v>256</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="122">
         <v>32</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="122">
         <v>2201</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="122">
         <v>5</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="122">
         <v>80</v>
       </c>
-      <c r="H9" s="121" t="s">
-        <v>69</v>
-      </c>
+      <c r="H9" s="105"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="122" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="122">
         <v>128</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="122">
         <v>36</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="122">
         <v>2201</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="122">
         <v>5</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="122">
         <v>315</v>
       </c>
-      <c r="H10" s="121" t="s">
-        <v>71</v>
-      </c>
+      <c r="H10" s="105"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" t="s">
-        <v>72</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="122" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="122">
         <v>128</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="122">
         <v>36</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="122">
         <v>2201</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="122">
         <v>5</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="122">
         <v>2200</v>
       </c>
-      <c r="H11" s="121" t="s">
-        <v>73</v>
-      </c>
+      <c r="H11" s="105"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" t="s">
+      <c r="B12" s="122" t="s">
         <v>50</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="122">
         <v>512</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="122">
         <v>128</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="122">
         <v>2290</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="122">
         <v>5</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="122">
         <v>896</v>
       </c>
-      <c r="H12" s="121" t="s">
-        <v>59</v>
+      <c r="H12" s="105"/>
+    </row>
+    <row r="13" spans="2:8">
+      <c r="B13" s="105" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H12" r:id="rId1" xr:uid="{A01791D3-3073-4C26-A28A-F8870BF61304}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{67CEC67E-AA78-4B77-BF18-5EE2186602EF}"/>
-    <hyperlink ref="H6" r:id="rId3" xr:uid="{2948ED0D-3DFD-4E50-99EE-8268D7972C3E}"/>
-    <hyperlink ref="H7" r:id="rId4" xr:uid="{2C4778B1-C813-4548-B266-69990239141B}"/>
-    <hyperlink ref="H8" r:id="rId5" xr:uid="{B1A9CC0F-3D08-4CD6-817B-FF1713E7F03C}"/>
-    <hyperlink ref="H9" r:id="rId6" xr:uid="{8DEF828D-DE2A-4129-B1E8-7D8C99742396}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{E6CBC808-C61F-4773-8E3B-D686655F98AF}"/>
-    <hyperlink ref="H11" r:id="rId8" xr:uid="{DF7B6B5F-867F-4487-B6F3-FF6B3EAB9E63}"/>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{CBD9B6A3-4FEB-42C9-AEE3-2B32B08D2CF8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId9"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6015E65F-B2D0-4CF9-825D-EC42022F84A6}">
-  <dimension ref="B2:G7"/>
+  <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4330,20 +4266,20 @@
       <c r="B6" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="103">
-        <v>18.8</v>
-      </c>
-      <c r="D6" s="103">
-        <v>17.8</v>
-      </c>
-      <c r="E6" s="103">
-        <v>17</v>
-      </c>
-      <c r="F6" s="103">
-        <v>16.7</v>
-      </c>
-      <c r="G6" s="103">
-        <v>11.8</v>
+      <c r="C6" s="104">
+        <v>0.188</v>
+      </c>
+      <c r="D6" s="104">
+        <v>0.17800000000000002</v>
+      </c>
+      <c r="E6" s="104">
+        <v>0.17</v>
+      </c>
+      <c r="F6" s="104">
+        <v>0.16699999999999998</v>
+      </c>
+      <c r="G6" s="104">
+        <v>0.11800000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:7">
@@ -4364,6 +4300,12 @@
       </c>
       <c r="G7" s="104">
         <v>0.22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="C9" s="104">
+        <f>SUM(C6:G6)</f>
+        <v>0.82100000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -4422,26 +4364,26 @@
         <v>28</v>
       </c>
       <c r="O4" s="109"/>
-      <c r="P4" s="106" t="s">
+      <c r="P4" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="107"/>
-      <c r="R4" s="106" t="s">
+      <c r="Q4" s="120"/>
+      <c r="R4" s="119" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="107"/>
-      <c r="T4" s="106" t="s">
+      <c r="S4" s="120"/>
+      <c r="T4" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="107"/>
-      <c r="V4" s="106" t="s">
+      <c r="U4" s="120"/>
+      <c r="V4" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="107"/>
-      <c r="Y4" s="106" t="s">
+      <c r="W4" s="120"/>
+      <c r="Y4" s="119" t="s">
         <v>31</v>
       </c>
-      <c r="Z4" s="107"/>
+      <c r="Z4" s="120"/>
     </row>
     <row r="5" spans="2:27">
       <c r="D5" s="1"/>
@@ -4483,10 +4425,10 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B7" s="110" t="s">
+      <c r="B7" s="115" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="118" t="s">
+      <c r="C7" s="112" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="69"/>
@@ -4515,8 +4457,8 @@
       <c r="AA7" s="3"/>
     </row>
     <row r="8" spans="2:27">
-      <c r="B8" s="111"/>
-      <c r="C8" s="118"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="112"/>
       <c r="D8" s="73"/>
       <c r="E8" s="74"/>
       <c r="F8" s="75"/>
@@ -4543,10 +4485,10 @@
       <c r="AA8" s="3"/>
     </row>
     <row r="9" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B9" s="112" t="s">
+      <c r="B9" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="119" t="s">
+      <c r="C9" s="113" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="14"/>
@@ -4575,8 +4517,8 @@
       <c r="AA9" s="3"/>
     </row>
     <row r="10" spans="2:27">
-      <c r="B10" s="113"/>
-      <c r="C10" s="119"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="113"/>
       <c r="D10" s="14"/>
       <c r="E10" s="19" t="s">
         <v>5</v>
@@ -4611,8 +4553,8 @@
       <c r="AA10" s="3"/>
     </row>
     <row r="11" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B11" s="113"/>
-      <c r="C11" s="119" t="s">
+      <c r="B11" s="118"/>
+      <c r="C11" s="113" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="14"/>
@@ -4641,8 +4583,8 @@
       <c r="AA11" s="3"/>
     </row>
     <row r="12" spans="2:27">
-      <c r="B12" s="113"/>
-      <c r="C12" s="119"/>
+      <c r="B12" s="118"/>
+      <c r="C12" s="113"/>
       <c r="D12" s="14"/>
       <c r="E12" s="17"/>
       <c r="F12" s="16"/>
@@ -4677,8 +4619,8 @@
       <c r="AA12" s="3"/>
     </row>
     <row r="13" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B13" s="113"/>
-      <c r="C13" s="120" t="s">
+      <c r="B13" s="118"/>
+      <c r="C13" s="114" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="14"/>
@@ -4707,8 +4649,8 @@
       <c r="AA13" s="3"/>
     </row>
     <row r="14" spans="2:27" ht="30">
-      <c r="B14" s="113"/>
-      <c r="C14" s="119"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="113"/>
       <c r="D14" s="14"/>
       <c r="E14" s="17"/>
       <c r="F14" s="16"/>
@@ -4751,10 +4693,10 @@
       <c r="AA14" s="3"/>
     </row>
     <row r="15" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B15" s="114" t="s">
+      <c r="B15" s="106" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="116" t="s">
+      <c r="C15" s="110" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="82"/>
@@ -4783,8 +4725,8 @@
       <c r="AA15" s="3"/>
     </row>
     <row r="16" spans="2:27" ht="16.5">
-      <c r="B16" s="115"/>
-      <c r="C16" s="117"/>
+      <c r="B16" s="107"/>
+      <c r="C16" s="111"/>
       <c r="D16" s="86"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
@@ -4823,8 +4765,8 @@
       <c r="AA16" s="3"/>
     </row>
     <row r="17" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B17" s="115"/>
-      <c r="C17" s="116" t="s">
+      <c r="B17" s="107"/>
+      <c r="C17" s="110" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="86"/>
@@ -4853,8 +4795,8 @@
       <c r="AA17" s="3"/>
     </row>
     <row r="18" spans="2:27" ht="16.5">
-      <c r="B18" s="115"/>
-      <c r="C18" s="117"/>
+      <c r="B18" s="107"/>
+      <c r="C18" s="111"/>
       <c r="D18" s="86"/>
       <c r="E18" s="29"/>
       <c r="F18" s="30"/>
@@ -4893,8 +4835,8 @@
       <c r="AA18" s="3"/>
     </row>
     <row r="19" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B19" s="115"/>
-      <c r="C19" s="116" t="s">
+      <c r="B19" s="107"/>
+      <c r="C19" s="110" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="86"/>
@@ -4923,8 +4865,8 @@
       <c r="AA19" s="3"/>
     </row>
     <row r="20" spans="2:27" ht="16.5">
-      <c r="B20" s="115"/>
-      <c r="C20" s="117"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="111"/>
       <c r="D20" s="87"/>
       <c r="E20" s="88" t="s">
         <v>5</v>
@@ -5033,10 +4975,10 @@
         <v>32</v>
       </c>
       <c r="D25" s="13"/>
-      <c r="E25" s="105" t="s">
+      <c r="E25" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="105"/>
+      <c r="I25" s="121"/>
       <c r="AA25" s="3"/>
     </row>
     <row r="26" spans="2:27">
@@ -5044,44 +4986,60 @@
         <v>33</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="105"/>
-      <c r="I26" s="105"/>
+      <c r="E26" s="121"/>
+      <c r="I26" s="121"/>
     </row>
     <row r="27" spans="2:27" ht="15.75" thickBot="1">
       <c r="B27" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="98"/>
-      <c r="E27" s="105" t="s">
+      <c r="E27" s="121" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="105"/>
+      <c r="I27" s="121"/>
     </row>
     <row r="28" spans="2:27">
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="99"/>
-      <c r="E28" s="105"/>
-      <c r="I28" s="105"/>
+      <c r="E28" s="121"/>
+      <c r="I28" s="121"/>
     </row>
     <row r="29" spans="2:27" ht="15.75" thickBot="1">
       <c r="B29" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="100"/>
-      <c r="E29" s="105" t="s">
+      <c r="E29" s="121" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="105"/>
+      <c r="I29" s="121"/>
     </row>
     <row r="30" spans="2:27">
       <c r="D30" s="101"/>
-      <c r="E30" s="105"/>
-      <c r="I30" s="105"/>
+      <c r="E30" s="121"/>
+      <c r="I30" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B14"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
@@ -5092,22 +5050,6 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B14"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[10-issue0005_ucv03] Update README and Part1.1 overall.
</commit_message>
<xml_diff>
--- a/Resources/README/README_Resources.xlsx
+++ b/Resources/README/README_Resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_dev\Repository\CSC_MS\Resources\README\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F1E24D-332A-4F07-97D0-DAE6884A97D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFA792A-959E-4B49-BCEB-3901B881C8AF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13545" xr2:uid="{5FC90DE4-2FBD-4B96-ADE9-01AE3F36C35E}"/>
   </bookViews>
@@ -258,7 +258,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +347,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1003,7 +1019,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1316,18 +1332,54 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="3">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1341,36 +1393,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3990,7 +4012,7 @@
   <dimension ref="B2:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4005,210 +4027,210 @@
       </c>
     </row>
     <row r="3" spans="2:8" ht="30">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="107" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="124" t="s">
+      <c r="C3" s="108" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="124" t="s">
+      <c r="D3" s="108" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="124" t="s">
+      <c r="E3" s="108" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="124" t="s">
+      <c r="F3" s="108" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="123" t="s">
+      <c r="G3" s="107" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:8">
-      <c r="B4" s="122" t="s">
+      <c r="B4" s="106" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="122">
+      <c r="C4" s="106">
         <v>32</v>
       </c>
-      <c r="D4" s="122">
+      <c r="D4" s="106">
         <v>12</v>
       </c>
-      <c r="E4" s="122">
+      <c r="E4" s="109">
         <v>2197</v>
       </c>
-      <c r="F4" s="122">
+      <c r="F4" s="106">
         <v>5</v>
       </c>
-      <c r="G4" s="122">
+      <c r="G4" s="106">
         <v>584</v>
       </c>
       <c r="H4" s="105"/>
     </row>
     <row r="5" spans="2:8">
-      <c r="B5" s="122" t="s">
+      <c r="B5" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="122">
+      <c r="C5" s="106">
         <v>128</v>
       </c>
-      <c r="D5" s="122">
+      <c r="D5" s="106">
         <v>24</v>
       </c>
-      <c r="E5" s="122">
+      <c r="E5" s="106">
         <v>2242</v>
       </c>
-      <c r="F5" s="122">
+      <c r="F5" s="106">
         <v>5</v>
       </c>
-      <c r="G5" s="122">
+      <c r="G5" s="106">
         <v>136</v>
       </c>
       <c r="H5" s="105"/>
     </row>
     <row r="6" spans="2:8">
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="106" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="122">
+      <c r="C6" s="106">
         <v>64</v>
       </c>
-      <c r="D6" s="122">
+      <c r="D6" s="106">
         <v>8</v>
       </c>
-      <c r="E6" s="122">
+      <c r="E6" s="106">
         <v>2201</v>
       </c>
-      <c r="F6" s="122">
+      <c r="F6" s="106">
         <v>5</v>
       </c>
-      <c r="G6" s="122">
+      <c r="G6" s="106">
         <v>663</v>
       </c>
       <c r="H6" s="105"/>
     </row>
     <row r="7" spans="2:8">
-      <c r="B7" s="122" t="s">
+      <c r="B7" s="106" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="122">
+      <c r="C7" s="106">
         <v>128</v>
       </c>
-      <c r="D7" s="122">
+      <c r="D7" s="106">
         <v>16</v>
       </c>
-      <c r="E7" s="122">
+      <c r="E7" s="106">
         <v>2201</v>
       </c>
-      <c r="F7" s="122">
+      <c r="F7" s="106">
         <v>5</v>
       </c>
-      <c r="G7" s="122">
+      <c r="G7" s="106">
         <v>71</v>
       </c>
       <c r="H7" s="105"/>
     </row>
     <row r="8" spans="2:8">
-      <c r="B8" s="122" t="s">
+      <c r="B8" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="122">
+      <c r="C8" s="106">
         <v>128</v>
       </c>
-      <c r="D8" s="122">
+      <c r="D8" s="106">
         <v>16</v>
       </c>
-      <c r="E8" s="122">
+      <c r="E8" s="106">
         <v>2201</v>
       </c>
-      <c r="F8" s="122">
+      <c r="F8" s="106">
         <v>5</v>
       </c>
-      <c r="G8" s="122">
+      <c r="G8" s="106">
         <v>304</v>
       </c>
       <c r="H8" s="105"/>
     </row>
     <row r="9" spans="2:8">
-      <c r="B9" s="122" t="s">
+      <c r="B9" s="106" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="122">
+      <c r="C9" s="106">
         <v>256</v>
       </c>
-      <c r="D9" s="122">
+      <c r="D9" s="106">
         <v>32</v>
       </c>
-      <c r="E9" s="122">
+      <c r="E9" s="106">
         <v>2201</v>
       </c>
-      <c r="F9" s="122">
+      <c r="F9" s="106">
         <v>5</v>
       </c>
-      <c r="G9" s="122">
+      <c r="G9" s="106">
         <v>80</v>
       </c>
       <c r="H9" s="105"/>
     </row>
     <row r="10" spans="2:8">
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="106" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="122">
+      <c r="C10" s="106">
         <v>128</v>
       </c>
-      <c r="D10" s="122">
+      <c r="D10" s="106">
         <v>36</v>
       </c>
-      <c r="E10" s="122">
+      <c r="E10" s="106">
         <v>2201</v>
       </c>
-      <c r="F10" s="122">
+      <c r="F10" s="106">
         <v>5</v>
       </c>
-      <c r="G10" s="122">
+      <c r="G10" s="106">
         <v>315</v>
       </c>
       <c r="H10" s="105"/>
     </row>
     <row r="11" spans="2:8">
-      <c r="B11" s="122" t="s">
+      <c r="B11" s="106" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="122">
+      <c r="C11" s="106">
         <v>128</v>
       </c>
-      <c r="D11" s="122">
+      <c r="D11" s="106">
         <v>36</v>
       </c>
-      <c r="E11" s="122">
+      <c r="E11" s="106">
         <v>2201</v>
       </c>
-      <c r="F11" s="122">
+      <c r="F11" s="106">
         <v>5</v>
       </c>
-      <c r="G11" s="122">
+      <c r="G11" s="109">
         <v>2200</v>
       </c>
       <c r="H11" s="105"/>
     </row>
     <row r="12" spans="2:8">
-      <c r="B12" s="122" t="s">
+      <c r="B12" s="109" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="122">
+      <c r="C12" s="110">
         <v>512</v>
       </c>
-      <c r="D12" s="122">
+      <c r="D12" s="110">
         <v>128</v>
       </c>
-      <c r="E12" s="122">
+      <c r="E12" s="106">
         <v>2290</v>
       </c>
-      <c r="F12" s="122">
+      <c r="F12" s="106">
         <v>5</v>
       </c>
-      <c r="G12" s="122">
+      <c r="G12" s="106">
         <v>896</v>
       </c>
       <c r="H12" s="105"/>
@@ -4344,46 +4366,46 @@
     </row>
     <row r="4" spans="2:27" ht="32.25" customHeight="1">
       <c r="D4" s="6"/>
-      <c r="E4" s="108" t="s">
+      <c r="E4" s="114" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="109"/>
-      <c r="G4" s="108" t="s">
+      <c r="F4" s="115"/>
+      <c r="G4" s="114" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="109"/>
-      <c r="I4" s="108" t="s">
+      <c r="H4" s="115"/>
+      <c r="I4" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="109"/>
-      <c r="K4" s="108" t="s">
+      <c r="J4" s="115"/>
+      <c r="K4" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="109"/>
-      <c r="N4" s="108" t="s">
+      <c r="L4" s="115"/>
+      <c r="N4" s="114" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="109"/>
-      <c r="P4" s="119" t="s">
+      <c r="O4" s="115"/>
+      <c r="P4" s="112" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="120"/>
-      <c r="R4" s="119" t="s">
+      <c r="Q4" s="113"/>
+      <c r="R4" s="112" t="s">
         <v>17</v>
       </c>
-      <c r="S4" s="120"/>
-      <c r="T4" s="119" t="s">
+      <c r="S4" s="113"/>
+      <c r="T4" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="U4" s="120"/>
-      <c r="V4" s="119" t="s">
+      <c r="U4" s="113"/>
+      <c r="V4" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="W4" s="120"/>
-      <c r="Y4" s="119" t="s">
+      <c r="W4" s="113"/>
+      <c r="Y4" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="Z4" s="120"/>
+      <c r="Z4" s="113"/>
     </row>
     <row r="5" spans="2:27">
       <c r="D5" s="1"/>
@@ -4425,10 +4447,10 @@
       <c r="Z6" s="4"/>
     </row>
     <row r="7" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B7" s="115" t="s">
+      <c r="B7" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C7" s="124" t="s">
         <v>0</v>
       </c>
       <c r="D7" s="69"/>
@@ -4457,8 +4479,8 @@
       <c r="AA7" s="3"/>
     </row>
     <row r="8" spans="2:27">
-      <c r="B8" s="116"/>
-      <c r="C8" s="112"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="124"/>
       <c r="D8" s="73"/>
       <c r="E8" s="74"/>
       <c r="F8" s="75"/>
@@ -4485,10 +4507,10 @@
       <c r="AA8" s="3"/>
     </row>
     <row r="9" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B9" s="117" t="s">
+      <c r="B9" s="118" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="113" t="s">
+      <c r="C9" s="125" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="14"/>
@@ -4517,8 +4539,8 @@
       <c r="AA9" s="3"/>
     </row>
     <row r="10" spans="2:27">
-      <c r="B10" s="118"/>
-      <c r="C10" s="113"/>
+      <c r="B10" s="119"/>
+      <c r="C10" s="125"/>
       <c r="D10" s="14"/>
       <c r="E10" s="19" t="s">
         <v>5</v>
@@ -4553,8 +4575,8 @@
       <c r="AA10" s="3"/>
     </row>
     <row r="11" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B11" s="118"/>
-      <c r="C11" s="113" t="s">
+      <c r="B11" s="119"/>
+      <c r="C11" s="125" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="14"/>
@@ -4583,8 +4605,8 @@
       <c r="AA11" s="3"/>
     </row>
     <row r="12" spans="2:27">
-      <c r="B12" s="118"/>
-      <c r="C12" s="113"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="125"/>
       <c r="D12" s="14"/>
       <c r="E12" s="17"/>
       <c r="F12" s="16"/>
@@ -4619,8 +4641,8 @@
       <c r="AA12" s="3"/>
     </row>
     <row r="13" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B13" s="118"/>
-      <c r="C13" s="114" t="s">
+      <c r="B13" s="119"/>
+      <c r="C13" s="126" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="14"/>
@@ -4649,8 +4671,8 @@
       <c r="AA13" s="3"/>
     </row>
     <row r="14" spans="2:27" ht="30">
-      <c r="B14" s="118"/>
-      <c r="C14" s="113"/>
+      <c r="B14" s="119"/>
+      <c r="C14" s="125"/>
       <c r="D14" s="14"/>
       <c r="E14" s="17"/>
       <c r="F14" s="16"/>
@@ -4693,10 +4715,10 @@
       <c r="AA14" s="3"/>
     </row>
     <row r="15" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B15" s="106" t="s">
+      <c r="B15" s="120" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="110" t="s">
+      <c r="C15" s="122" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="82"/>
@@ -4725,8 +4747,8 @@
       <c r="AA15" s="3"/>
     </row>
     <row r="16" spans="2:27" ht="16.5">
-      <c r="B16" s="107"/>
-      <c r="C16" s="111"/>
+      <c r="B16" s="121"/>
+      <c r="C16" s="123"/>
       <c r="D16" s="86"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
@@ -4765,8 +4787,8 @@
       <c r="AA16" s="3"/>
     </row>
     <row r="17" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B17" s="107"/>
-      <c r="C17" s="110" t="s">
+      <c r="B17" s="121"/>
+      <c r="C17" s="122" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="86"/>
@@ -4795,8 +4817,8 @@
       <c r="AA17" s="3"/>
     </row>
     <row r="18" spans="2:27" ht="16.5">
-      <c r="B18" s="107"/>
-      <c r="C18" s="111"/>
+      <c r="B18" s="121"/>
+      <c r="C18" s="123"/>
       <c r="D18" s="86"/>
       <c r="E18" s="29"/>
       <c r="F18" s="30"/>
@@ -4835,8 +4857,8 @@
       <c r="AA18" s="3"/>
     </row>
     <row r="19" spans="2:27" ht="15.75" thickBot="1">
-      <c r="B19" s="107"/>
-      <c r="C19" s="110" t="s">
+      <c r="B19" s="121"/>
+      <c r="C19" s="122" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="86"/>
@@ -4865,8 +4887,8 @@
       <c r="AA19" s="3"/>
     </row>
     <row r="20" spans="2:27" ht="16.5">
-      <c r="B20" s="107"/>
-      <c r="C20" s="111"/>
+      <c r="B20" s="121"/>
+      <c r="C20" s="123"/>
       <c r="D20" s="87"/>
       <c r="E20" s="88" t="s">
         <v>5</v>
@@ -4975,10 +4997,10 @@
         <v>32</v>
       </c>
       <c r="D25" s="13"/>
-      <c r="E25" s="121" t="s">
+      <c r="E25" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="121"/>
+      <c r="I25" s="111"/>
       <c r="AA25" s="3"/>
     </row>
     <row r="26" spans="2:27">
@@ -4986,60 +5008,44 @@
         <v>33</v>
       </c>
       <c r="D26" s="10"/>
-      <c r="E26" s="121"/>
-      <c r="I26" s="121"/>
+      <c r="E26" s="111"/>
+      <c r="I26" s="111"/>
     </row>
     <row r="27" spans="2:27" ht="15.75" thickBot="1">
       <c r="B27" t="s">
         <v>34</v>
       </c>
       <c r="D27" s="98"/>
-      <c r="E27" s="121" t="s">
+      <c r="E27" s="111" t="s">
         <v>38</v>
       </c>
-      <c r="I27" s="121"/>
+      <c r="I27" s="111"/>
     </row>
     <row r="28" spans="2:27">
       <c r="B28" t="s">
         <v>35</v>
       </c>
       <c r="D28" s="99"/>
-      <c r="E28" s="121"/>
-      <c r="I28" s="121"/>
+      <c r="E28" s="111"/>
+      <c r="I28" s="111"/>
     </row>
     <row r="29" spans="2:27" ht="15.75" thickBot="1">
       <c r="B29" t="s">
         <v>36</v>
       </c>
       <c r="D29" s="100"/>
-      <c r="E29" s="121" t="s">
+      <c r="E29" s="111" t="s">
         <v>39</v>
       </c>
-      <c r="I29" s="121"/>
+      <c r="I29" s="111"/>
     </row>
     <row r="30" spans="2:27">
       <c r="D30" s="101"/>
-      <c r="E30" s="121"/>
-      <c r="I30" s="121"/>
+      <c r="E30" s="111"/>
+      <c r="I30" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="R4:S4"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B9:B14"/>
     <mergeCell ref="B15:B20"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
@@ -5050,6 +5056,22 @@
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="C17:C18"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B9:B14"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:S4"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="E29:E30"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>